<commit_message>
Se agregan estilos al archivo excel
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -16,7 +16,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Yaears Experience</t>
+    <t>Years of Experience</t>
   </si>
   <si>
     <t>Category</t>
@@ -59,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -67,16 +67,24 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA500"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -84,12 +92,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,16 +453,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>